<commit_message>
Updated EDA file and created a report
</commit_message>
<xml_diff>
--- a/All_data_correct.xlsx
+++ b/All_data_correct.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1Emilias Data\1Publications\2024\Monica e Leandro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monii\OneDrive\Escritorio\PersonalityAndTeamClimate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94687121-7DC4-4CB4-A39F-7506705FCFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DA589F-CC7A-40B5-8F5B-F41CE018330E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2F6CBA60-D0A4-46F3-A9E5-1391D28D06B3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2F6CBA60-D0A4-46F3-A9E5-1391D28D06B3}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="2" r:id="rId1"/>
@@ -1636,7 +1636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1673,6 +1673,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1973,7 +1974,18 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE2CF777-72B2-4C22-BF33-68D03419ED73}" name="Ericsson_Karlskrona_2018" displayName="Ericsson_Karlskrona_2018" ref="A1:BB283" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:BB283" xr:uid="{EE2CF777-72B2-4C22-BF33-68D03419ED73}"/>
+  <autoFilter ref="A1:BB283" xr:uid="{EE2CF777-72B2-4C22-BF33-68D03419ED73}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Male"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="8">
+      <filters>
+        <filter val="India"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="54">
     <tableColumn id="1" xr3:uid="{3DA2799E-37B2-48B6-9D07-6E0C03F55E3F}" uniqueName="1" name="Ericsson location" queryTableFieldId="1" dataDxfId="23"/>
     <tableColumn id="2" xr3:uid="{486C80D9-64BD-4365-B576-6DB15B1B6643}" uniqueName="2" name="Participant ID" queryTableFieldId="2" dataDxfId="22"/>
@@ -2035,7 +2047,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -2333,43 +2345,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502ED652-260C-4582-84B8-25239A67FD53}">
   <dimension ref="A1:BB283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F134" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H166" sqref="H166"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I147" sqref="I147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="13.44140625" customWidth="1"/>
-    <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="15.44140625" customWidth="1"/>
-    <col min="24" max="24" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="18.6640625" customWidth="1"/>
-    <col min="31" max="31" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="37" width="13.33203125" customWidth="1"/>
-    <col min="38" max="38" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="45" width="11.44140625" customWidth="1"/>
-    <col min="46" max="46" width="17.6640625" customWidth="1"/>
-    <col min="47" max="47" width="23.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="13.42578125" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="15.42578125" customWidth="1"/>
+    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="18.7109375" customWidth="1"/>
+    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="37" width="13.28515625" customWidth="1"/>
+    <col min="38" max="38" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="45" width="11.42578125" customWidth="1"/>
+    <col min="46" max="46" width="17.7109375" customWidth="1"/>
+    <col min="47" max="47" width="23.7109375" customWidth="1"/>
     <col min="48" max="48" width="20" customWidth="1"/>
-    <col min="49" max="49" width="15.77734375" customWidth="1"/>
-    <col min="50" max="50" width="20.109375" customWidth="1"/>
-    <col min="51" max="51" width="21.77734375" customWidth="1"/>
-    <col min="52" max="52" width="15.109375" customWidth="1"/>
-    <col min="53" max="53" width="18.109375" customWidth="1"/>
-    <col min="54" max="54" width="28.6640625" customWidth="1"/>
+    <col min="49" max="49" width="15.7109375" customWidth="1"/>
+    <col min="50" max="50" width="20.140625" customWidth="1"/>
+    <col min="51" max="51" width="21.7109375" customWidth="1"/>
+    <col min="52" max="52" width="15.140625" customWidth="1"/>
+    <col min="53" max="53" width="18.140625" customWidth="1"/>
+    <col min="54" max="54" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2533,7 +2545,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2682,7 +2694,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2831,7 +2843,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2980,7 +2992,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -3129,7 +3141,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3278,7 +3290,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3427,7 +3439,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -3576,7 +3588,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3725,7 +3737,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3874,7 +3886,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -4023,7 +4035,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -4172,7 +4184,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -4321,7 +4333,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -4470,7 +4482,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -4619,7 +4631,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -4768,7 +4780,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -4917,7 +4929,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -5066,7 +5078,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -5215,7 +5227,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -5364,7 +5376,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -5513,7 +5525,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -5662,7 +5674,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -5811,7 +5823,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -5960,7 +5972,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -6109,7 +6121,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -6258,7 +6270,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -6407,7 +6419,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -6556,7 +6568,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -6705,7 +6717,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -6854,7 +6866,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -7003,7 +7015,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:49" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -7152,7 +7164,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="33" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -7301,7 +7313,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -7450,7 +7462,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -7599,7 +7611,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -7748,7 +7760,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -7897,7 +7909,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -8046,7 +8058,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -8195,7 +8207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -8344,7 +8356,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -8493,7 +8505,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -8642,7 +8654,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -8791,7 +8803,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="44" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -8940,7 +8952,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>231</v>
       </c>
@@ -9098,7 +9110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
         <v>231</v>
       </c>
@@ -9256,7 +9268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
         <v>231</v>
       </c>
@@ -9414,7 +9426,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
         <v>231</v>
       </c>
@@ -9572,7 +9584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C49" s="2" t="s">
         <v>231</v>
       </c>
@@ -9730,7 +9742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
         <v>231</v>
       </c>
@@ -9888,7 +9900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
         <v>231</v>
       </c>
@@ -10046,7 +10058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
         <v>231</v>
       </c>
@@ -10204,7 +10216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C53" s="2" t="s">
         <v>231</v>
       </c>
@@ -10362,7 +10374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
         <v>231</v>
       </c>
@@ -10520,7 +10532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C55" s="2" t="s">
         <v>231</v>
       </c>
@@ -10678,7 +10690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
         <v>231</v>
       </c>
@@ -10836,7 +10848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>231</v>
       </c>
@@ -10994,7 +11006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C58" s="1" t="s">
         <v>231</v>
       </c>
@@ -11152,7 +11164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C59" s="2" t="s">
         <v>231</v>
       </c>
@@ -11310,7 +11322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C60" s="1" t="s">
         <v>231</v>
       </c>
@@ -11468,7 +11480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C61" s="2" t="s">
         <v>231</v>
       </c>
@@ -11626,7 +11638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C62" s="2" t="s">
         <v>231</v>
       </c>
@@ -11784,7 +11796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
         <v>231</v>
       </c>
@@ -11942,7 +11954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C64" s="1" t="s">
         <v>231</v>
       </c>
@@ -12100,7 +12112,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
         <v>231</v>
       </c>
@@ -12258,7 +12270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
         <v>231</v>
       </c>
@@ -12416,7 +12428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C67" s="2" t="s">
         <v>231</v>
       </c>
@@ -12574,7 +12586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C68" s="1" t="s">
         <v>231</v>
       </c>
@@ -12732,7 +12744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
         <v>231</v>
       </c>
@@ -12890,7 +12902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
         <v>231</v>
       </c>
@@ -13048,7 +13060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C71" s="2" t="s">
         <v>231</v>
       </c>
@@ -13206,7 +13218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C72" s="2" t="s">
         <v>231</v>
       </c>
@@ -13364,7 +13376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
         <v>231</v>
       </c>
@@ -13522,7 +13534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C74" s="2" t="s">
         <v>231</v>
       </c>
@@ -13680,7 +13692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C75" s="1" t="s">
         <v>231</v>
       </c>
@@ -13838,7 +13850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="2" t="s">
         <v>231</v>
       </c>
@@ -13996,7 +14008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C77" s="1" t="s">
         <v>231</v>
       </c>
@@ -14154,7 +14166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C78" s="1" t="s">
         <v>231</v>
       </c>
@@ -14312,7 +14324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C79" s="1" t="s">
         <v>231</v>
       </c>
@@ -14470,7 +14482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C80" s="1" t="s">
         <v>231</v>
       </c>
@@ -14628,7 +14640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C81" s="2" t="s">
         <v>231</v>
       </c>
@@ -14786,7 +14798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C82" s="1" t="s">
         <v>231</v>
       </c>
@@ -14944,7 +14956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C83" s="2" t="s">
         <v>231</v>
       </c>
@@ -15102,7 +15114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C84" s="2" t="s">
         <v>231</v>
       </c>
@@ -15260,7 +15272,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C85" s="2" t="s">
         <v>231</v>
       </c>
@@ -15418,7 +15430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C86" s="1" t="s">
         <v>231</v>
       </c>
@@ -15576,7 +15588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C87" s="2" t="s">
         <v>231</v>
       </c>
@@ -15734,7 +15746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C88" s="2" t="s">
         <v>231</v>
       </c>
@@ -15892,7 +15904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C89" s="1" t="s">
         <v>231</v>
       </c>
@@ -16050,7 +16062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C90" s="2" t="s">
         <v>231</v>
       </c>
@@ -16208,7 +16220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C91" s="2" t="s">
         <v>231</v>
       </c>
@@ -16366,7 +16378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C92" s="2" t="s">
         <v>231</v>
       </c>
@@ -16524,7 +16536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C93" s="2" t="s">
         <v>231</v>
       </c>
@@ -16682,7 +16694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C94" s="2" t="s">
         <v>231</v>
       </c>
@@ -16840,7 +16852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C95" s="2" t="s">
         <v>231</v>
       </c>
@@ -16998,7 +17010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C96" s="1" t="s">
         <v>231</v>
       </c>
@@ -17156,7 +17168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C97" s="1" t="s">
         <v>231</v>
       </c>
@@ -17314,7 +17326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C98" s="2" t="s">
         <v>231</v>
       </c>
@@ -17472,7 +17484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
         <v>231</v>
       </c>
@@ -17630,7 +17642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C100" s="2" t="s">
         <v>231</v>
       </c>
@@ -17788,7 +17800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C101" s="1" t="s">
         <v>231</v>
       </c>
@@ -17947,7 +17959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C102" s="2" t="s">
         <v>231</v>
       </c>
@@ -18105,7 +18117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C103" s="1" t="s">
         <v>231</v>
       </c>
@@ -18263,7 +18275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C104" s="2" t="s">
         <v>231</v>
       </c>
@@ -18421,7 +18433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C105" s="2" t="s">
         <v>231</v>
       </c>
@@ -18579,7 +18591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C106" s="2" t="s">
         <v>231</v>
       </c>
@@ -18737,7 +18749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C107" s="1" t="s">
         <v>231</v>
       </c>
@@ -18895,7 +18907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C108" s="1" t="s">
         <v>231</v>
       </c>
@@ -19053,7 +19065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C109" s="2" t="s">
         <v>231</v>
       </c>
@@ -19211,7 +19223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C110" s="1" t="s">
         <v>231</v>
       </c>
@@ -19369,7 +19381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C111" s="2" t="s">
         <v>231</v>
       </c>
@@ -19527,7 +19539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C112" s="1" t="s">
         <v>231</v>
       </c>
@@ -19685,7 +19697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C113" s="2" t="s">
         <v>231</v>
       </c>
@@ -19843,7 +19855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C114" s="1" t="s">
         <v>231</v>
       </c>
@@ -20001,7 +20013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C115" s="1" t="s">
         <v>231</v>
       </c>
@@ -20159,7 +20171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C116" s="2" t="s">
         <v>231</v>
       </c>
@@ -20317,7 +20329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C117" s="1" t="s">
         <v>231</v>
       </c>
@@ -20475,7 +20487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C118" s="1" t="s">
         <v>231</v>
       </c>
@@ -20633,7 +20645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
         <v>348</v>
       </c>
@@ -20791,7 +20803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C120" t="s">
         <v>348</v>
       </c>
@@ -20949,7 +20961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
         <v>348</v>
       </c>
@@ -21107,7 +21119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
         <v>348</v>
       </c>
@@ -21265,7 +21277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
         <v>348</v>
       </c>
@@ -21285,7 +21297,7 @@
         <v>365</v>
       </c>
       <c r="I123" t="s">
-        <v>378</v>
+        <v>90</v>
       </c>
       <c r="J123">
         <v>80</v>
@@ -21423,7 +21435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
         <v>348</v>
       </c>
@@ -21581,7 +21593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C125" t="s">
         <v>348</v>
       </c>
@@ -21739,7 +21751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
         <v>348</v>
       </c>
@@ -21897,7 +21909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C127" t="s">
         <v>348</v>
       </c>
@@ -22055,7 +22067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C128" t="s">
         <v>348</v>
       </c>
@@ -22213,7 +22225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C129" t="s">
         <v>348</v>
       </c>
@@ -22371,7 +22383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C130" t="s">
         <v>348</v>
       </c>
@@ -22529,7 +22541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C131" t="s">
         <v>348</v>
       </c>
@@ -22687,7 +22699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C132" t="s">
         <v>348</v>
       </c>
@@ -22845,7 +22857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C133" t="s">
         <v>348</v>
       </c>
@@ -23003,7 +23015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C134" t="s">
         <v>348</v>
       </c>
@@ -23161,7 +23173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
         <v>348</v>
       </c>
@@ -23319,7 +23331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C136" t="s">
         <v>348</v>
       </c>
@@ -23477,7 +23489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
         <v>348</v>
       </c>
@@ -23635,7 +23647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="138" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
         <v>348</v>
       </c>
@@ -23793,7 +23805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="139" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C139" t="s">
         <v>348</v>
       </c>
@@ -23951,7 +23963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="140" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C140" t="s">
         <v>348</v>
       </c>
@@ -23971,7 +23983,7 @@
         <v>362</v>
       </c>
       <c r="I140" t="s">
-        <v>378</v>
+        <v>90</v>
       </c>
       <c r="J140">
         <v>50</v>
@@ -24109,7 +24121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="141" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C141" t="s">
         <v>348</v>
       </c>
@@ -24267,7 +24279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C142" t="s">
         <v>348</v>
       </c>
@@ -24425,7 +24437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="143" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C143" t="s">
         <v>348</v>
       </c>
@@ -24583,7 +24595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="144" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C144" t="s">
         <v>348</v>
       </c>
@@ -24603,7 +24615,7 @@
         <v>374</v>
       </c>
       <c r="I144" t="s">
-        <v>378</v>
+        <v>90</v>
       </c>
       <c r="J144">
         <v>95</v>
@@ -24741,7 +24753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="145" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C145" t="s">
         <v>348</v>
       </c>
@@ -24899,7 +24911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="146" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C146" t="s">
         <v>348</v>
       </c>
@@ -25057,7 +25069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="147" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C147" t="s">
         <v>348</v>
       </c>
@@ -25076,7 +25088,7 @@
       <c r="H147" t="s">
         <v>361</v>
       </c>
-      <c r="I147" t="s">
+      <c r="I147" s="20" t="s">
         <v>90</v>
       </c>
       <c r="J147">
@@ -25215,7 +25227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="148" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C148" t="s">
         <v>348</v>
       </c>
@@ -25373,7 +25385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="149" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C149" t="s">
         <v>348</v>
       </c>
@@ -25531,7 +25543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="150" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C150" t="s">
         <v>348</v>
       </c>
@@ -25689,7 +25701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="151" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C151" t="s">
         <v>348</v>
       </c>
@@ -25847,7 +25859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="152" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C152" t="s">
         <v>348</v>
       </c>
@@ -26005,7 +26017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="153" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C153" t="s">
         <v>348</v>
       </c>
@@ -26163,7 +26175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="154" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C154" t="s">
         <v>348</v>
       </c>
@@ -26321,7 +26333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="155" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C155" t="s">
         <v>348</v>
       </c>
@@ -26479,7 +26491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="156" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C156" t="s">
         <v>348</v>
       </c>
@@ -26637,7 +26649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="157" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C157" t="s">
         <v>348</v>
       </c>
@@ -26795,7 +26807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="158" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C158" t="s">
         <v>348</v>
       </c>
@@ -26953,7 +26965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="159" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C159" t="s">
         <v>348</v>
       </c>
@@ -26973,7 +26985,7 @@
         <v>361</v>
       </c>
       <c r="I159" t="s">
-        <v>378</v>
+        <v>90</v>
       </c>
       <c r="J159">
         <v>12</v>
@@ -27111,7 +27123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="160" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
         <v>348</v>
       </c>
@@ -27269,7 +27281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="161" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C161" t="s">
         <v>348</v>
       </c>
@@ -27427,7 +27439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="162" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C162" t="s">
         <v>348</v>
       </c>
@@ -27585,7 +27597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="163" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C163" t="s">
         <v>348</v>
       </c>
@@ -27743,7 +27755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="164" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C164" t="s">
         <v>348</v>
       </c>
@@ -27901,7 +27913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="165" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C165" t="s">
         <v>382</v>
       </c>
@@ -28059,7 +28071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="166" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C166" t="s">
         <v>382</v>
       </c>
@@ -28217,7 +28229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="167" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C167" t="s">
         <v>382</v>
       </c>
@@ -28375,7 +28387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="168" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C168" t="s">
         <v>382</v>
       </c>
@@ -28533,7 +28545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="169" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C169" t="s">
         <v>382</v>
       </c>
@@ -28691,7 +28703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="170" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C170" t="s">
         <v>382</v>
       </c>
@@ -28849,7 +28861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="171" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C171" t="s">
         <v>382</v>
       </c>
@@ -29007,7 +29019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="172" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C172" t="s">
         <v>382</v>
       </c>
@@ -29165,7 +29177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="173" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C173" t="s">
         <v>382</v>
       </c>
@@ -29323,7 +29335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="174" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C174" t="s">
         <v>382</v>
       </c>
@@ -29481,7 +29493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="175" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C175" t="s">
         <v>382</v>
       </c>
@@ -29639,7 +29651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="176" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C176" t="s">
         <v>382</v>
       </c>
@@ -29797,7 +29809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="177" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C177" t="s">
         <v>382</v>
       </c>
@@ -29955,7 +29967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="178" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C178" t="s">
         <v>382</v>
       </c>
@@ -30113,7 +30125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="179" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C179" t="s">
         <v>382</v>
       </c>
@@ -30271,7 +30283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="180" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C180" t="s">
         <v>382</v>
       </c>
@@ -30429,7 +30441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="181" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C181" t="s">
         <v>382</v>
       </c>
@@ -30587,7 +30599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="182" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C182" t="s">
         <v>382</v>
       </c>
@@ -30745,7 +30757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="183" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C183" t="s">
         <v>382</v>
       </c>
@@ -30903,7 +30915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="184" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C184" t="s">
         <v>382</v>
       </c>
@@ -31061,7 +31073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="185" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C185" t="s">
         <v>382</v>
       </c>
@@ -31219,7 +31231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="186" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C186" t="s">
         <v>382</v>
       </c>
@@ -31377,7 +31389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="187" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C187" t="s">
         <v>382</v>
       </c>
@@ -31535,7 +31547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="188" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C188" t="s">
         <v>382</v>
       </c>
@@ -31693,7 +31705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="189" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C189" t="s">
         <v>382</v>
       </c>
@@ -31851,7 +31863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="190" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C190" t="s">
         <v>382</v>
       </c>
@@ -32009,7 +32021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="191" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C191" t="s">
         <v>382</v>
       </c>
@@ -32167,7 +32179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="192" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C192" t="s">
         <v>382</v>
       </c>
@@ -32325,7 +32337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="193" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C193" t="s">
         <v>382</v>
       </c>
@@ -32483,7 +32495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="194" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C194" t="s">
         <v>382</v>
       </c>
@@ -32641,7 +32653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="195" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C195" t="s">
         <v>382</v>
       </c>
@@ -32799,7 +32811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="196" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C196" t="s">
         <v>382</v>
       </c>
@@ -32957,7 +32969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="197" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C197" t="s">
         <v>382</v>
       </c>
@@ -33115,7 +33127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="198" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C198" t="s">
         <v>382</v>
       </c>
@@ -33273,7 +33285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="199" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C199" t="s">
         <v>382</v>
       </c>
@@ -33431,7 +33443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="200" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C200" t="s">
         <v>382</v>
       </c>
@@ -33589,7 +33601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="201" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C201" t="s">
         <v>382</v>
       </c>
@@ -33747,7 +33759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="202" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C202" t="s">
         <v>382</v>
       </c>
@@ -33905,7 +33917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="203" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C203" t="s">
         <v>382</v>
       </c>
@@ -34063,7 +34075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="204" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C204" t="s">
         <v>382</v>
       </c>
@@ -34221,7 +34233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="205" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C205" t="s">
         <v>382</v>
       </c>
@@ -34379,7 +34391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="206" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C206" t="s">
         <v>382</v>
       </c>
@@ -34537,7 +34549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="207" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C207" t="s">
         <v>382</v>
       </c>
@@ -34695,7 +34707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="208" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C208" t="s">
         <v>382</v>
       </c>
@@ -34853,7 +34865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="209" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C209" t="s">
         <v>382</v>
       </c>
@@ -35011,7 +35023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="210" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C210" t="s">
         <v>382</v>
       </c>
@@ -35169,7 +35181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="211" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C211" t="s">
         <v>382</v>
       </c>
@@ -35327,7 +35339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="212" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C212" t="s">
         <v>382</v>
       </c>
@@ -35485,7 +35497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="213" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C213" t="s">
         <v>382</v>
       </c>
@@ -35643,7 +35655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="214" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C214" t="s">
         <v>382</v>
       </c>
@@ -35801,7 +35813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="215" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C215" t="s">
         <v>382</v>
       </c>
@@ -35959,7 +35971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="216" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C216" t="s">
         <v>382</v>
       </c>
@@ -36117,7 +36129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="217" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C217" t="s">
         <v>382</v>
       </c>
@@ -36275,7 +36287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="218" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C218" t="s">
         <v>382</v>
       </c>
@@ -36433,7 +36445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="219" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C219" t="s">
         <v>382</v>
       </c>
@@ -36591,7 +36603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="220" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C220" t="s">
         <v>382</v>
       </c>
@@ -36749,7 +36761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="221" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C221" t="s">
         <v>382</v>
       </c>
@@ -36907,7 +36919,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="222" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C222" t="s">
         <v>382</v>
       </c>
@@ -37065,7 +37077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="223" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="223" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C223" t="s">
         <v>382</v>
       </c>
@@ -37223,7 +37235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="224" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C224" t="s">
         <v>382</v>
       </c>
@@ -37381,7 +37393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="225" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C225" t="s">
         <v>382</v>
       </c>
@@ -37539,7 +37551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="226" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C226" t="s">
         <v>382</v>
       </c>
@@ -37697,7 +37709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="227" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C227" t="s">
         <v>382</v>
       </c>
@@ -37855,7 +37867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="228" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C228" t="s">
         <v>382</v>
       </c>
@@ -38013,7 +38025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="229" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="229" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C229" t="s">
         <v>382</v>
       </c>
@@ -38171,7 +38183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="230" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C230" t="s">
         <v>382</v>
       </c>
@@ -38329,7 +38341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="231" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C231" t="s">
         <v>382</v>
       </c>
@@ -38487,7 +38499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="232" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C232" t="s">
         <v>382</v>
       </c>
@@ -38645,7 +38657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="233" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C233" t="s">
         <v>382</v>
       </c>
@@ -38803,7 +38815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="234" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C234" t="s">
         <v>382</v>
       </c>
@@ -38961,7 +38973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="235" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C235" t="s">
         <v>382</v>
       </c>
@@ -39119,7 +39131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="236" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C236" t="s">
         <v>382</v>
       </c>
@@ -39277,7 +39289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="237" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C237" t="s">
         <v>382</v>
       </c>
@@ -39435,7 +39447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="238" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C238" t="s">
         <v>382</v>
       </c>
@@ -39593,7 +39605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="239" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C239" t="s">
         <v>382</v>
       </c>
@@ -39751,7 +39763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="240" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C240" t="s">
         <v>382</v>
       </c>
@@ -39909,7 +39921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="241" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C241" t="s">
         <v>382</v>
       </c>
@@ -40067,7 +40079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="242" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C242" t="s">
         <v>382</v>
       </c>
@@ -40225,7 +40237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="243" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C243" t="s">
         <v>382</v>
       </c>
@@ -40383,7 +40395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="244" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C244" t="s">
         <v>382</v>
       </c>
@@ -40541,7 +40553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="245" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C245" t="s">
         <v>382</v>
       </c>
@@ -40699,7 +40711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="246" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C246" t="s">
         <v>382</v>
       </c>
@@ -40857,7 +40869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="247" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C247" t="s">
         <v>382</v>
       </c>
@@ -41015,7 +41027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="248" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C248" t="s">
         <v>382</v>
       </c>
@@ -41173,7 +41185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="249" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C249" t="s">
         <v>382</v>
       </c>
@@ -41331,7 +41343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="250" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C250" t="s">
         <v>382</v>
       </c>
@@ -41489,7 +41501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="251" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="251" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C251" t="s">
         <v>382</v>
       </c>
@@ -41647,7 +41659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="252" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C252" t="s">
         <v>382</v>
       </c>
@@ -41805,7 +41817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="253" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C253" t="s">
         <v>382</v>
       </c>
@@ -41963,7 +41975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="254" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C254" t="s">
         <v>382</v>
       </c>
@@ -42121,7 +42133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="255" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="255" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C255" t="s">
         <v>382</v>
       </c>
@@ -42279,7 +42291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="256" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="256" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C256" t="s">
         <v>382</v>
       </c>
@@ -42437,7 +42449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="257" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C257" t="s">
         <v>382</v>
       </c>
@@ -42595,7 +42607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="258" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C258" t="s">
         <v>382</v>
       </c>
@@ -42753,7 +42765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="259" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C259" t="s">
         <v>382</v>
       </c>
@@ -42911,7 +42923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="260" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C260" t="s">
         <v>382</v>
       </c>
@@ -43069,7 +43081,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="261" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C261" t="s">
         <v>382</v>
       </c>
@@ -43227,7 +43239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="262" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C262" t="s">
         <v>382</v>
       </c>
@@ -43385,7 +43397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="263" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C263" t="s">
         <v>382</v>
       </c>
@@ -43543,7 +43555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="264" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C264" t="s">
         <v>382</v>
       </c>
@@ -43701,7 +43713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="265" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C265" t="s">
         <v>382</v>
       </c>
@@ -43859,7 +43871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="266" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C266" t="s">
         <v>382</v>
       </c>
@@ -44017,7 +44029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="267" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C267" t="s">
         <v>382</v>
       </c>
@@ -44175,7 +44187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="268" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="268" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C268" t="s">
         <v>382</v>
       </c>
@@ -44333,7 +44345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="269" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C269" t="s">
         <v>382</v>
       </c>
@@ -44491,7 +44503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="270" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C270" t="s">
         <v>382</v>
       </c>
@@ -44649,7 +44661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="271" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="271" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C271" t="s">
         <v>382</v>
       </c>
@@ -44807,7 +44819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="272" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="272" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C272" t="s">
         <v>382</v>
       </c>
@@ -44965,7 +44977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="273" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C273" t="s">
         <v>382</v>
       </c>
@@ -45123,7 +45135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="274" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C274" t="s">
         <v>382</v>
       </c>
@@ -45281,7 +45293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="275" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="275" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C275" t="s">
         <v>382</v>
       </c>
@@ -45439,7 +45451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="276" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C276" t="s">
         <v>382</v>
       </c>
@@ -45597,7 +45609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="277" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="277" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C277" t="s">
         <v>382</v>
       </c>
@@ -45755,7 +45767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="278" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="278" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C278" t="s">
         <v>382</v>
       </c>
@@ -45913,7 +45925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="279" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C279" t="s">
         <v>382</v>
       </c>
@@ -46071,7 +46083,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="280" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="280" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C280" t="s">
         <v>382</v>
       </c>
@@ -46229,7 +46241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="281" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="281" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C281" t="s">
         <v>382</v>
       </c>
@@ -46387,7 +46399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="282" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="282" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C282" t="s">
         <v>382</v>
       </c>
@@ -46545,7 +46557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="283" spans="3:54" x14ac:dyDescent="0.3">
+    <row r="283" spans="3:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="C283" t="s">
         <v>382</v>
       </c>
@@ -46719,7 +46731,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -46733,9 +46745,9 @@
       <selection activeCell="A75" sqref="A1:BE75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -46790,7 +46802,7 @@
       <c r="AZ1" s="1"/>
       <c r="BA1" s="1"/>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -46845,7 +46857,7 @@
       <c r="AZ2" s="2"/>
       <c r="BA2" s="2"/>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -46900,7 +46912,7 @@
       <c r="AZ3" s="1"/>
       <c r="BA3" s="1"/>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -46955,7 +46967,7 @@
       <c r="AZ4" s="2"/>
       <c r="BA4" s="2"/>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -47010,7 +47022,7 @@
       <c r="AZ5" s="2"/>
       <c r="BA5" s="2"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -47065,7 +47077,7 @@
       <c r="AZ6" s="2"/>
       <c r="BA6" s="2"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -47120,7 +47132,7 @@
       <c r="AZ7" s="1"/>
       <c r="BA7" s="1"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -47175,7 +47187,7 @@
       <c r="AZ8" s="1"/>
       <c r="BA8" s="1"/>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -47230,7 +47242,7 @@
       <c r="AZ9" s="2"/>
       <c r="BA9" s="2"/>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -47285,7 +47297,7 @@
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -47340,7 +47352,7 @@
       <c r="AZ11" s="2"/>
       <c r="BA11" s="2"/>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -47395,7 +47407,7 @@
       <c r="AZ12" s="1"/>
       <c r="BA12" s="1"/>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -47450,7 +47462,7 @@
       <c r="AZ13" s="2"/>
       <c r="BA13" s="2"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -47505,7 +47517,7 @@
       <c r="AZ14" s="1"/>
       <c r="BA14" s="1"/>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -47560,7 +47572,7 @@
       <c r="AZ15" s="2"/>
       <c r="BA15" s="2"/>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -47615,7 +47627,7 @@
       <c r="AZ16" s="1"/>
       <c r="BA16" s="1"/>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -47670,7 +47682,7 @@
       <c r="AZ17" s="2"/>
       <c r="BA17" s="2"/>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -47725,7 +47737,7 @@
       <c r="AZ18" s="2"/>
       <c r="BA18" s="2"/>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -47780,7 +47792,7 @@
       <c r="AZ19" s="1"/>
       <c r="BA19" s="1"/>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -47835,7 +47847,7 @@
       <c r="AZ20" s="1"/>
       <c r="BA20" s="1"/>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -47890,7 +47902,7 @@
       <c r="AZ21" s="1"/>
       <c r="BA21" s="1"/>
     </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -47945,7 +47957,7 @@
       <c r="AZ22" s="1"/>
       <c r="BA22" s="1"/>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -48000,7 +48012,7 @@
       <c r="AZ23" s="2"/>
       <c r="BA23" s="2"/>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -48055,7 +48067,7 @@
       <c r="AZ24" s="1"/>
       <c r="BA24" s="1"/>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -48110,7 +48122,7 @@
       <c r="AZ25" s="1"/>
       <c r="BA25" s="1"/>
     </row>
-    <row r="26" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -48165,7 +48177,7 @@
       <c r="AZ26" s="1"/>
       <c r="BA26" s="1"/>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -48220,7 +48232,7 @@
       <c r="AZ27" s="2"/>
       <c r="BA27" s="2"/>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -48275,7 +48287,7 @@
       <c r="AZ28" s="2"/>
       <c r="BA28" s="2"/>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -48330,7 +48342,7 @@
       <c r="AZ29" s="1"/>
       <c r="BA29" s="1"/>
     </row>
-    <row r="30" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -48385,7 +48397,7 @@
       <c r="AZ30" s="2"/>
       <c r="BA30" s="2"/>
     </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -48440,7 +48452,7 @@
       <c r="AZ31" s="1"/>
       <c r="BA31" s="1"/>
     </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -48495,7 +48507,7 @@
       <c r="AZ32" s="2"/>
       <c r="BA32" s="2"/>
     </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -48550,7 +48562,7 @@
       <c r="AZ33" s="1"/>
       <c r="BA33" s="1"/>
     </row>
-    <row r="34" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -48605,7 +48617,7 @@
       <c r="AZ34" s="1"/>
       <c r="BA34" s="1"/>
     </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -48660,7 +48672,7 @@
       <c r="AZ35" s="1"/>
       <c r="BA35" s="1"/>
     </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -48715,7 +48727,7 @@
       <c r="AZ36" s="1"/>
       <c r="BA36" s="1"/>
     </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -48770,7 +48782,7 @@
       <c r="AZ37" s="2"/>
       <c r="BA37" s="2"/>
     </row>
-    <row r="38" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -48825,7 +48837,7 @@
       <c r="AZ38" s="1"/>
       <c r="BA38" s="1"/>
     </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -48880,7 +48892,7 @@
       <c r="AZ39" s="2"/>
       <c r="BA39" s="2"/>
     </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -48935,7 +48947,7 @@
       <c r="AZ40" s="2"/>
       <c r="BA40" s="2"/>
     </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -48990,7 +49002,7 @@
       <c r="AZ41" s="2"/>
       <c r="BA41" s="2"/>
     </row>
-    <row r="42" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -49045,7 +49057,7 @@
       <c r="AZ42" s="1"/>
       <c r="BA42" s="1"/>
     </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -49100,7 +49112,7 @@
       <c r="AZ43" s="2"/>
       <c r="BA43" s="2"/>
     </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -49155,7 +49167,7 @@
       <c r="AZ44" s="2"/>
       <c r="BA44" s="2"/>
     </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -49210,7 +49222,7 @@
       <c r="AZ45" s="1"/>
       <c r="BA45" s="1"/>
     </row>
-    <row r="46" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -49265,7 +49277,7 @@
       <c r="AZ46" s="2"/>
       <c r="BA46" s="2"/>
     </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -49320,7 +49332,7 @@
       <c r="AZ47" s="2"/>
       <c r="BA47" s="2"/>
     </row>
-    <row r="48" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -49375,7 +49387,7 @@
       <c r="AZ48" s="2"/>
       <c r="BA48" s="2"/>
     </row>
-    <row r="49" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -49430,7 +49442,7 @@
       <c r="AZ49" s="1"/>
       <c r="BA49" s="1"/>
     </row>
-    <row r="50" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -49485,7 +49497,7 @@
       <c r="AZ50" s="2"/>
       <c r="BA50" s="2"/>
     </row>
-    <row r="51" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -49540,7 +49552,7 @@
       <c r="AZ51" s="2"/>
       <c r="BA51" s="2"/>
     </row>
-    <row r="52" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -49595,7 +49607,7 @@
       <c r="AZ52" s="2"/>
       <c r="BA52" s="2"/>
     </row>
-    <row r="53" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -49650,7 +49662,7 @@
       <c r="AZ53" s="1"/>
       <c r="BA53" s="1"/>
     </row>
-    <row r="54" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -49705,7 +49717,7 @@
       <c r="AZ54" s="1"/>
       <c r="BA54" s="1"/>
     </row>
-    <row r="55" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -49760,7 +49772,7 @@
       <c r="AZ55" s="2"/>
       <c r="BA55" s="2"/>
     </row>
-    <row r="56" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -49815,7 +49827,7 @@
       <c r="AZ56" s="1"/>
       <c r="BA56" s="1"/>
     </row>
-    <row r="57" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -49870,7 +49882,7 @@
       <c r="AZ57" s="2"/>
       <c r="BA57" s="2"/>
     </row>
-    <row r="58" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -49925,7 +49937,7 @@
       <c r="AZ58" s="1"/>
       <c r="BA58" s="1"/>
     </row>
-    <row r="59" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -49980,7 +49992,7 @@
       <c r="AZ59" s="2"/>
       <c r="BA59" s="2"/>
     </row>
-    <row r="60" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -50035,7 +50047,7 @@
       <c r="AZ60" s="1"/>
       <c r="BA60" s="1"/>
     </row>
-    <row r="61" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -50090,7 +50102,7 @@
       <c r="AZ61" s="2"/>
       <c r="BA61" s="2"/>
     </row>
-    <row r="62" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -50145,7 +50157,7 @@
       <c r="AZ62" s="2"/>
       <c r="BA62" s="2"/>
     </row>
-    <row r="63" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -50200,7 +50212,7 @@
       <c r="AZ63" s="2"/>
       <c r="BA63" s="2"/>
     </row>
-    <row r="64" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -50255,7 +50267,7 @@
       <c r="AZ64" s="1"/>
       <c r="BA64" s="1"/>
     </row>
-    <row r="65" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -50310,7 +50322,7 @@
       <c r="AZ65" s="1"/>
       <c r="BA65" s="1"/>
     </row>
-    <row r="66" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -50365,7 +50377,7 @@
       <c r="AZ66" s="2"/>
       <c r="BA66" s="2"/>
     </row>
-    <row r="67" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -50420,7 +50432,7 @@
       <c r="AZ67" s="1"/>
       <c r="BA67" s="1"/>
     </row>
-    <row r="68" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -50475,7 +50487,7 @@
       <c r="AZ68" s="2"/>
       <c r="BA68" s="2"/>
     </row>
-    <row r="69" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -50530,7 +50542,7 @@
       <c r="AZ69" s="1"/>
       <c r="BA69" s="1"/>
     </row>
-    <row r="70" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -50585,7 +50597,7 @@
       <c r="AZ70" s="2"/>
       <c r="BA70" s="2"/>
     </row>
-    <row r="71" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -50640,7 +50652,7 @@
       <c r="AZ71" s="1"/>
       <c r="BA71" s="1"/>
     </row>
-    <row r="72" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -50695,7 +50707,7 @@
       <c r="AZ72" s="1"/>
       <c r="BA72" s="1"/>
     </row>
-    <row r="73" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -50750,7 +50762,7 @@
       <c r="AZ73" s="2"/>
       <c r="BA73" s="2"/>
     </row>
-    <row r="74" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -50805,7 +50817,7 @@
       <c r="AZ74" s="1"/>
       <c r="BA74" s="1"/>
     </row>
-    <row r="75" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -50876,17 +50888,17 @@
       <selection sqref="A1:M151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="19.109375" style="17" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" style="17" customWidth="1"/>
-    <col min="9" max="9" width="8.77734375" style="17"/>
-    <col min="10" max="10" width="12.77734375" style="17" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" style="17" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="17"/>
+    <col min="10" max="10" width="12.7109375" style="17" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="17" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="11"/>
@@ -50895,7 +50907,7 @@
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="12"/>
@@ -50904,7 +50916,7 @@
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="11"/>
@@ -50913,7 +50925,7 @@
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="12"/>
@@ -50922,7 +50934,7 @@
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="11"/>
@@ -50931,7 +50943,7 @@
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="12"/>
@@ -50940,7 +50952,7 @@
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="11"/>
@@ -50949,7 +50961,7 @@
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="12"/>
@@ -50958,7 +50970,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="11"/>
@@ -50967,7 +50979,7 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="12"/>
@@ -50976,7 +50988,7 @@
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="11"/>
@@ -50985,7 +50997,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="12"/>
@@ -50994,7 +51006,7 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="11"/>
@@ -51003,7 +51015,7 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="12"/>
@@ -51012,7 +51024,7 @@
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="11"/>
@@ -51021,7 +51033,7 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="12"/>
@@ -51030,7 +51042,7 @@
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="11"/>
@@ -51039,7 +51051,7 @@
       <c r="I17" s="16"/>
       <c r="J17" s="16"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="12"/>
@@ -51048,7 +51060,7 @@
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="11"/>
@@ -51057,7 +51069,7 @@
       <c r="I19" s="16"/>
       <c r="J19" s="16"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="12"/>
@@ -51066,7 +51078,7 @@
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="11"/>
@@ -51075,7 +51087,7 @@
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="12"/>
@@ -51084,7 +51096,7 @@
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="11"/>
@@ -51093,7 +51105,7 @@
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="12"/>
@@ -51102,7 +51114,7 @@
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="11"/>
@@ -51111,7 +51123,7 @@
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="12"/>
@@ -51120,7 +51132,7 @@
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="11"/>
@@ -51129,7 +51141,7 @@
       <c r="I27" s="16"/>
       <c r="J27" s="16"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="12"/>
@@ -51138,7 +51150,7 @@
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="11"/>
@@ -51147,7 +51159,7 @@
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="12"/>
@@ -51156,7 +51168,7 @@
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="11"/>
@@ -51165,7 +51177,7 @@
       <c r="I31" s="16"/>
       <c r="J31" s="16"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="12"/>
@@ -51174,7 +51186,7 @@
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="11"/>
@@ -51183,7 +51195,7 @@
       <c r="I33" s="16"/>
       <c r="J33" s="16"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="12"/>
@@ -51192,7 +51204,7 @@
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="11"/>
@@ -51201,7 +51213,7 @@
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="12"/>
@@ -51210,7 +51222,7 @@
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="11"/>
@@ -51219,7 +51231,7 @@
       <c r="I37" s="16"/>
       <c r="J37" s="16"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="12"/>
@@ -51228,7 +51240,7 @@
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="11"/>
@@ -51237,7 +51249,7 @@
       <c r="I39" s="16"/>
       <c r="J39" s="16"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="12"/>
@@ -51246,7 +51258,7 @@
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="11"/>
@@ -51255,7 +51267,7 @@
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="12"/>
@@ -51264,7 +51276,7 @@
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="11"/>
@@ -51273,7 +51285,7 @@
       <c r="I43" s="16"/>
       <c r="J43" s="16"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="12"/>
@@ -51282,7 +51294,7 @@
       <c r="I44" s="18"/>
       <c r="J44" s="18"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="11"/>
@@ -51291,7 +51303,7 @@
       <c r="I45" s="16"/>
       <c r="J45" s="16"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="12"/>
@@ -51300,7 +51312,7 @@
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="11"/>
@@ -51309,7 +51321,7 @@
       <c r="I47" s="16"/>
       <c r="J47" s="16"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="13"/>
@@ -51318,7 +51330,7 @@
       <c r="I48" s="18"/>
       <c r="J48" s="18"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="11"/>
@@ -51327,7 +51339,7 @@
       <c r="I49" s="16"/>
       <c r="J49" s="16"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="C50" s="12"/>
@@ -51336,7 +51348,7 @@
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="11"/>
@@ -51345,7 +51357,7 @@
       <c r="I51" s="16"/>
       <c r="J51" s="16"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="12"/>
@@ -51354,7 +51366,7 @@
       <c r="I52" s="18"/>
       <c r="J52" s="18"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="11"/>
@@ -51363,7 +51375,7 @@
       <c r="I53" s="16"/>
       <c r="J53" s="16"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="12"/>
@@ -51372,7 +51384,7 @@
       <c r="I54" s="18"/>
       <c r="J54" s="18"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="11"/>
@@ -51381,7 +51393,7 @@
       <c r="I55" s="16"/>
       <c r="J55" s="16"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="12"/>
@@ -51390,7 +51402,7 @@
       <c r="I56" s="18"/>
       <c r="J56" s="18"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="11"/>
@@ -51399,7 +51411,7 @@
       <c r="I57" s="16"/>
       <c r="J57" s="16"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="12"/>
@@ -51408,7 +51420,7 @@
       <c r="I58" s="18"/>
       <c r="J58" s="18"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="11"/>
@@ -51417,7 +51429,7 @@
       <c r="I59" s="16"/>
       <c r="J59" s="16"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="12"/>
@@ -51426,7 +51438,7 @@
       <c r="I60" s="18"/>
       <c r="J60" s="18"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="11"/>
@@ -51435,7 +51447,7 @@
       <c r="I61" s="16"/>
       <c r="J61" s="16"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="C62" s="12"/>
@@ -51444,7 +51456,7 @@
       <c r="I62" s="18"/>
       <c r="J62" s="18"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="11"/>
@@ -51453,7 +51465,7 @@
       <c r="I63" s="16"/>
       <c r="J63" s="16"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="12"/>
@@ -51462,7 +51474,7 @@
       <c r="I64" s="18"/>
       <c r="J64" s="18"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="11"/>
@@ -51471,7 +51483,7 @@
       <c r="I65" s="16"/>
       <c r="J65" s="16"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="C66" s="12"/>
@@ -51480,7 +51492,7 @@
       <c r="I66" s="18"/>
       <c r="J66" s="18"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="11"/>
@@ -51489,7 +51501,7 @@
       <c r="I67" s="16"/>
       <c r="J67" s="16"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="C68" s="12"/>
@@ -51498,7 +51510,7 @@
       <c r="I68" s="18"/>
       <c r="J68" s="18"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="11"/>
@@ -51507,7 +51519,7 @@
       <c r="I69" s="16"/>
       <c r="J69" s="16"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="C70" s="12"/>
@@ -51516,7 +51528,7 @@
       <c r="I70" s="18"/>
       <c r="J70" s="18"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="11"/>
@@ -51525,7 +51537,7 @@
       <c r="I71" s="16"/>
       <c r="J71" s="16"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="12"/>
@@ -51534,7 +51546,7 @@
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="11"/>
@@ -51543,7 +51555,7 @@
       <c r="I73" s="16"/>
       <c r="J73" s="16"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="12"/>
@@ -51552,7 +51564,7 @@
       <c r="I74" s="18"/>
       <c r="J74" s="18"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="G75" s="16"/>
@@ -51560,439 +51572,439 @@
       <c r="I75" s="16"/>
       <c r="J75" s="16"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G76" s="18"/>
       <c r="H76" s="18"/>
       <c r="I76" s="18"/>
       <c r="J76" s="18"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G77" s="16"/>
       <c r="H77" s="16"/>
       <c r="I77" s="16"/>
       <c r="J77" s="16"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G78" s="18"/>
       <c r="H78" s="18"/>
       <c r="I78" s="18"/>
       <c r="J78" s="18"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G79" s="16"/>
       <c r="H79" s="16"/>
       <c r="I79" s="16"/>
       <c r="J79" s="16"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G80" s="18"/>
       <c r="H80" s="18"/>
       <c r="I80" s="18"/>
       <c r="J80" s="18"/>
     </row>
-    <row r="81" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G81" s="16"/>
       <c r="H81" s="16"/>
       <c r="I81" s="16"/>
       <c r="J81" s="16"/>
     </row>
-    <row r="82" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G82" s="18"/>
       <c r="H82" s="18"/>
       <c r="I82" s="18"/>
       <c r="J82" s="18"/>
     </row>
-    <row r="83" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G83" s="16"/>
       <c r="H83" s="16"/>
       <c r="I83" s="16"/>
       <c r="J83" s="16"/>
     </row>
-    <row r="84" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G84" s="18"/>
       <c r="H84" s="18"/>
       <c r="I84" s="18"/>
       <c r="J84" s="18"/>
     </row>
-    <row r="85" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G85" s="16"/>
       <c r="H85" s="16"/>
       <c r="I85" s="16"/>
       <c r="J85" s="16"/>
     </row>
-    <row r="86" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G86" s="18"/>
       <c r="H86" s="18"/>
       <c r="I86" s="18"/>
       <c r="J86" s="18"/>
     </row>
-    <row r="87" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G87" s="16"/>
       <c r="H87" s="16"/>
       <c r="I87" s="16"/>
       <c r="J87" s="16"/>
     </row>
-    <row r="88" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G88" s="18"/>
       <c r="H88" s="18"/>
       <c r="I88" s="18"/>
       <c r="J88" s="18"/>
     </row>
-    <row r="89" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G89" s="16"/>
       <c r="H89" s="16"/>
       <c r="I89" s="16"/>
       <c r="J89" s="16"/>
     </row>
-    <row r="90" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G90" s="18"/>
       <c r="H90" s="18"/>
       <c r="I90" s="18"/>
       <c r="J90" s="18"/>
     </row>
-    <row r="91" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G91" s="16"/>
       <c r="H91" s="16"/>
       <c r="I91" s="16"/>
       <c r="J91" s="16"/>
     </row>
-    <row r="92" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G92" s="18"/>
       <c r="H92" s="18"/>
       <c r="I92" s="18"/>
       <c r="J92" s="18"/>
     </row>
-    <row r="93" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G93" s="16"/>
       <c r="H93" s="16"/>
       <c r="I93" s="16"/>
       <c r="J93" s="16"/>
     </row>
-    <row r="94" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G94" s="18"/>
       <c r="H94" s="18"/>
       <c r="I94" s="18"/>
       <c r="J94" s="18"/>
     </row>
-    <row r="95" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G95" s="16"/>
       <c r="H95" s="16"/>
       <c r="I95" s="16"/>
       <c r="J95" s="16"/>
     </row>
-    <row r="96" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G96" s="18"/>
       <c r="H96" s="18"/>
       <c r="I96" s="18"/>
       <c r="J96" s="18"/>
     </row>
-    <row r="97" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G97" s="16"/>
       <c r="H97" s="16"/>
       <c r="I97" s="16"/>
       <c r="J97" s="16"/>
     </row>
-    <row r="98" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G98" s="18"/>
       <c r="H98" s="18"/>
       <c r="I98" s="18"/>
       <c r="J98" s="18"/>
     </row>
-    <row r="99" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G99" s="16"/>
       <c r="H99" s="18"/>
       <c r="I99" s="18"/>
       <c r="J99" s="18"/>
     </row>
-    <row r="100" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G100" s="18"/>
       <c r="H100" s="18"/>
       <c r="I100" s="18"/>
       <c r="J100" s="18"/>
     </row>
-    <row r="101" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G101" s="16"/>
       <c r="H101" s="16"/>
       <c r="I101" s="16"/>
       <c r="J101" s="16"/>
     </row>
-    <row r="102" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G102" s="18"/>
       <c r="H102" s="18"/>
       <c r="I102" s="18"/>
       <c r="J102" s="18"/>
     </row>
-    <row r="103" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G103" s="16"/>
       <c r="H103" s="18"/>
       <c r="I103" s="16"/>
       <c r="J103" s="16"/>
     </row>
-    <row r="104" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G104" s="18"/>
       <c r="H104" s="18"/>
       <c r="I104" s="18"/>
       <c r="J104" s="18"/>
     </row>
-    <row r="105" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G105" s="16"/>
       <c r="H105" s="16"/>
       <c r="I105" s="16"/>
       <c r="J105" s="16"/>
     </row>
-    <row r="106" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G106" s="18"/>
       <c r="H106" s="18"/>
       <c r="I106" s="18"/>
       <c r="J106" s="18"/>
     </row>
-    <row r="107" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G107" s="16"/>
       <c r="H107" s="16"/>
       <c r="I107" s="16"/>
       <c r="J107" s="16"/>
     </row>
-    <row r="108" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G108" s="18"/>
       <c r="H108" s="18"/>
       <c r="I108" s="18"/>
       <c r="J108" s="18"/>
     </row>
-    <row r="109" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G109" s="16"/>
       <c r="H109" s="16"/>
       <c r="I109" s="16"/>
       <c r="J109" s="16"/>
     </row>
-    <row r="110" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G110" s="18"/>
       <c r="H110" s="18"/>
       <c r="I110" s="18"/>
       <c r="J110" s="18"/>
     </row>
-    <row r="111" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G111" s="16"/>
       <c r="H111" s="18"/>
       <c r="I111" s="18"/>
       <c r="J111" s="16"/>
     </row>
-    <row r="112" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G112" s="18"/>
       <c r="H112" s="18"/>
       <c r="I112" s="18"/>
       <c r="J112" s="18"/>
     </row>
-    <row r="113" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G113" s="16"/>
       <c r="H113" s="16"/>
       <c r="I113" s="16"/>
       <c r="J113" s="16"/>
     </row>
-    <row r="114" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G114" s="18"/>
       <c r="H114" s="18"/>
       <c r="I114" s="18"/>
       <c r="J114" s="18"/>
     </row>
-    <row r="115" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G115" s="16"/>
       <c r="H115" s="16"/>
       <c r="I115" s="16"/>
       <c r="J115" s="16"/>
     </row>
-    <row r="116" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G116" s="18"/>
       <c r="H116" s="18"/>
       <c r="I116" s="18"/>
       <c r="J116" s="18"/>
     </row>
-    <row r="117" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G117" s="16"/>
       <c r="H117" s="16"/>
       <c r="I117" s="16"/>
       <c r="J117" s="16"/>
     </row>
-    <row r="118" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G118" s="18"/>
       <c r="H118" s="18"/>
       <c r="I118" s="18"/>
       <c r="J118" s="18"/>
     </row>
-    <row r="119" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G119" s="16"/>
       <c r="H119" s="16"/>
       <c r="I119" s="16"/>
       <c r="J119" s="16"/>
     </row>
-    <row r="120" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G120" s="18"/>
       <c r="H120" s="18"/>
       <c r="I120" s="18"/>
       <c r="J120" s="18"/>
     </row>
-    <row r="121" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G121" s="16"/>
       <c r="H121" s="16"/>
       <c r="I121" s="16"/>
       <c r="J121" s="16"/>
     </row>
-    <row r="122" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G122" s="18"/>
       <c r="H122" s="18"/>
       <c r="I122" s="18"/>
       <c r="J122" s="18"/>
     </row>
-    <row r="123" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G123" s="16"/>
       <c r="H123" s="16"/>
       <c r="I123" s="16"/>
       <c r="J123" s="16"/>
     </row>
-    <row r="124" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G124" s="18"/>
       <c r="H124" s="18"/>
       <c r="I124" s="18"/>
       <c r="J124" s="18"/>
     </row>
-    <row r="125" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G125" s="16"/>
       <c r="H125" s="16"/>
       <c r="I125" s="16"/>
       <c r="J125" s="16"/>
     </row>
-    <row r="126" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G126" s="18"/>
       <c r="H126" s="18"/>
       <c r="I126" s="18"/>
       <c r="J126" s="18"/>
     </row>
-    <row r="127" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G127" s="16"/>
       <c r="H127" s="16"/>
       <c r="I127" s="16"/>
       <c r="J127" s="16"/>
     </row>
-    <row r="128" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G128" s="18"/>
       <c r="H128" s="18"/>
       <c r="I128" s="18"/>
       <c r="J128" s="18"/>
     </row>
-    <row r="129" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G129" s="16"/>
       <c r="H129" s="16"/>
       <c r="I129" s="16"/>
       <c r="J129" s="16"/>
     </row>
-    <row r="130" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G130" s="18"/>
       <c r="H130" s="18"/>
       <c r="I130" s="18"/>
       <c r="J130" s="18"/>
     </row>
-    <row r="131" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G131" s="16"/>
       <c r="H131" s="16"/>
       <c r="I131" s="16"/>
       <c r="J131" s="16"/>
     </row>
-    <row r="132" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G132" s="18"/>
       <c r="H132" s="18"/>
       <c r="I132" s="18"/>
       <c r="J132" s="18"/>
     </row>
-    <row r="133" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G133" s="16"/>
       <c r="H133" s="16"/>
       <c r="I133" s="16"/>
       <c r="J133" s="16"/>
     </row>
-    <row r="134" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G134" s="18"/>
       <c r="H134" s="18"/>
       <c r="I134" s="18"/>
       <c r="J134" s="18"/>
     </row>
-    <row r="135" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G135" s="16"/>
       <c r="H135" s="16"/>
       <c r="I135" s="16"/>
       <c r="J135" s="16"/>
     </row>
-    <row r="136" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G136" s="18"/>
       <c r="H136" s="18"/>
       <c r="I136" s="18"/>
       <c r="J136" s="18"/>
     </row>
-    <row r="137" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G137" s="16"/>
       <c r="H137" s="16"/>
       <c r="I137" s="16"/>
       <c r="J137" s="16"/>
     </row>
-    <row r="138" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G138" s="18"/>
       <c r="H138" s="18"/>
       <c r="I138" s="18"/>
       <c r="J138" s="18"/>
     </row>
-    <row r="139" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G139" s="16"/>
       <c r="H139" s="16"/>
       <c r="I139" s="16"/>
       <c r="J139" s="16"/>
     </row>
-    <row r="140" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G140" s="18"/>
       <c r="H140" s="18"/>
       <c r="I140" s="18"/>
       <c r="J140" s="18"/>
     </row>
-    <row r="141" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G141" s="16"/>
       <c r="H141" s="16"/>
       <c r="I141" s="16"/>
       <c r="J141" s="16"/>
     </row>
-    <row r="142" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G142" s="18"/>
       <c r="H142" s="18"/>
       <c r="I142" s="18"/>
       <c r="J142" s="18"/>
     </row>
-    <row r="143" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G143" s="16"/>
       <c r="H143" s="16"/>
       <c r="I143" s="16"/>
       <c r="J143" s="16"/>
     </row>
-    <row r="144" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G144" s="18"/>
       <c r="H144" s="18"/>
       <c r="I144" s="18"/>
       <c r="J144" s="18"/>
     </row>
-    <row r="145" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G145" s="16"/>
       <c r="H145" s="16"/>
       <c r="I145" s="16"/>
       <c r="J145" s="16"/>
     </row>
-    <row r="146" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G146" s="18"/>
       <c r="H146" s="18"/>
       <c r="I146" s="18"/>
       <c r="J146" s="18"/>
     </row>
-    <row r="147" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G147" s="16"/>
       <c r="H147" s="16"/>
       <c r="I147" s="16"/>
       <c r="J147" s="16"/>
     </row>
-    <row r="148" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G148" s="18"/>
       <c r="H148" s="18"/>
       <c r="I148" s="18"/>

</xml_diff>